<commit_message>
Another round of runs
</commit_message>
<xml_diff>
--- a/service-compare-data/Data.xlsx
+++ b/service-compare-data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvinson\Documents\GitHub\StupidTodo\service-compare-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F215A6BE-F3F5-4C3E-8D2B-A9A1724F342A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A384B3EF-FF89-4FA9-BE9F-054346730E7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88F3D2B2-D218-436A-B106-F9482C8178E2}"/>
+    <workbookView xWindow="1845" yWindow="765" windowWidth="19665" windowHeight="12600" activeTab="4" xr2:uid="{88F3D2B2-D218-436A-B106-F9482C8178E2}"/>
   </bookViews>
   <sheets>
     <sheet name="GetChart" sheetId="2" r:id="rId1"/>
@@ -340,19 +340,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.73</c:v>
+                    <c:v>3.16</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.34</c:v>
+                    <c:v>1.77</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.58</c:v>
+                    <c:v>5.12</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.6</c:v>
+                    <c:v>3.36</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.5</c:v>
+                    <c:v>16.399999999999999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -364,19 +364,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.73</c:v>
+                    <c:v>3.16</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.34</c:v>
+                    <c:v>1.77</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.58</c:v>
+                    <c:v>5.12</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.6</c:v>
+                    <c:v>3.36</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.5</c:v>
+                    <c:v>16.399999999999999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -424,19 +424,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>33.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.6</c:v>
+                  <c:v>21.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.599999999999994</c:v>
+                  <c:v>73.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62</c:v>
+                  <c:v>54.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87.4</c:v>
+                  <c:v>72.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,19 +559,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>18.7</c:v>
+                    <c:v>15.7</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>38.4</c:v>
+                    <c:v>19.100000000000001</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.2</c:v>
+                    <c:v>228</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>14.5</c:v>
+                    <c:v>22.6</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>27.6</c:v>
+                    <c:v>31</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -583,19 +583,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>18.7</c:v>
+                    <c:v>15.7</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>38.4</c:v>
+                    <c:v>19.100000000000001</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.2</c:v>
+                    <c:v>228</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>14.5</c:v>
+                    <c:v>22.6</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>27.6</c:v>
+                    <c:v>31</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -643,19 +643,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>94.6</c:v>
+                  <c:v>80.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83</c:v>
+                  <c:v>66.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.400000000000006</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>174</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,6 +873,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1076,16 +1077,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>3.33</c:v>
+                    <c:v>4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.58</c:v>
+                    <c:v>2.33</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.77</c:v>
+                    <c:v>16.899999999999999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.62</c:v>
+                    <c:v>12.2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1097,16 +1098,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>3.33</c:v>
+                    <c:v>4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.58</c:v>
+                    <c:v>2.33</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.77</c:v>
+                    <c:v>16.899999999999999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.62</c:v>
+                    <c:v>12.2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1151,16 +1152,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>32.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.599999999999994</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.3</c:v>
+                  <c:v>75.099999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,16 +1284,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>11.2</c:v>
+                    <c:v>6.24</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>43.2</c:v>
+                    <c:v>16.399999999999999</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>35.4</c:v>
+                    <c:v>30</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>33.4</c:v>
+                    <c:v>23.2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1304,16 +1305,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>11.2</c:v>
+                    <c:v>6.24</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>43.2</c:v>
+                    <c:v>16.399999999999999</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>35.4</c:v>
+                    <c:v>30</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>33.4</c:v>
+                    <c:v>23.2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1358,16 +1359,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>73.400000000000006</c:v>
+                  <c:v>52.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.400000000000006</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>280</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>211</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1446,6 +1447,8 @@
         <c:axId val="555710255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="275"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1626,7 +1629,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Get 1 Todo (ms)</a:t>
+              <a:t>First Todo (Get</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 1)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> (ms)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1785,16 +1796,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>0.22</c:v>
+                    <c:v>0.28000000000000003</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.27</c:v>
+                    <c:v>0.18</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.26</c:v>
+                    <c:v>0.42</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.99</c:v>
+                    <c:v>2.2000000000000002</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1806,16 +1817,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>0.22</c:v>
+                    <c:v>0.28000000000000003</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.27</c:v>
+                    <c:v>0.18</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.26</c:v>
+                    <c:v>0.42</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.99</c:v>
+                    <c:v>2.2000000000000002</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1860,16 +1871,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.05</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>1.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.61</c:v>
+                  <c:v>1.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.47</c:v>
+                  <c:v>3.06</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1992,16 +2003,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>13.2</c:v>
+                    <c:v>1.04</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.65</c:v>
+                    <c:v>2.27</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.0500000000000007</c:v>
+                    <c:v>2.4700000000000002</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>16.100000000000001</c:v>
+                    <c:v>3.03</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2013,16 +2024,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>13.2</c:v>
+                    <c:v>1.04</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.65</c:v>
+                    <c:v>2.27</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.0500000000000007</c:v>
+                    <c:v>2.4700000000000002</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>16.100000000000001</c:v>
+                    <c:v>3.03</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2067,16 +2078,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>22.9</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8</c:v>
+                  <c:v>2.37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.15</c:v>
+                  <c:v>2.39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.2</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2155,7 +2166,7 @@
         <c:axId val="623189839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32"/>
+          <c:max val="6.5"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2496,16 +2507,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>0.72</c:v>
+                    <c:v>0.83</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.31</c:v>
+                    <c:v>0.18</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.78</c:v>
+                    <c:v>1.1200000000000001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.0599999999999996</c:v>
+                    <c:v>5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2517,16 +2528,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>0.72</c:v>
+                    <c:v>0.83</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.31</c:v>
+                    <c:v>0.18</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.78</c:v>
+                    <c:v>1.1200000000000001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.0599999999999996</c:v>
+                    <c:v>5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2571,16 +2582,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.11</c:v>
+                  <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.02</c:v>
+                  <c:v>7.91</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.15</c:v>
+                  <c:v>4.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2703,16 +2714,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>8.08</c:v>
+                    <c:v>4.6399999999999997</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.33</c:v>
+                    <c:v>1.94</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.92</c:v>
+                    <c:v>5.09</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.6</c:v>
+                    <c:v>2.56</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2724,16 +2735,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>8.08</c:v>
+                    <c:v>4.6399999999999997</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.33</c:v>
+                    <c:v>1.94</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.92</c:v>
+                    <c:v>5.09</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.6</c:v>
+                    <c:v>2.56</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2778,16 +2789,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>15.8</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.03</c:v>
+                  <c:v>1.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.600000000000001</c:v>
+                  <c:v>15.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.3</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2866,7 +2877,7 @@
         <c:axId val="623195663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="25"/>
+          <c:max val="21"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5144,7 +5155,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{768BB3DA-09A5-443B-B80C-D1A37A3B6DA0}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5155,7 +5166,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{506F3C1E-2D84-473D-9FC7-1F79AA6C7F61}">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5166,7 +5177,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{616AA3DE-0333-466A-955A-ABE1F5F27ADF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5177,7 +5188,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7E75149C-8DD5-444E-8BE1-A29C1C87BE8F}">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5188,7 +5199,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656320" cy="6278880"/>
+    <xdr:ext cx="8680739" cy="6299489"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5218,10 +5229,73 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.50249</cdr:x>
+      <cdr:y>0.09966</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.60599</cdr:x>
+      <cdr:y>0.1512</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46C8EACC-2B16-4CF9-BCED-F58BA4931FDA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4362018" y="627783"/>
+          <a:ext cx="898380" cy="324716"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>435</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> +/- 228</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:solidFill>
+              <a:schemeClr val="bg2"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656320" cy="6278880"/>
+    <xdr:ext cx="8659752" cy="6289408"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5250,11 +5324,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656320" cy="6278880"/>
+    <xdr:ext cx="8659752" cy="6289408"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5283,11 +5357,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656320" cy="6278880"/>
+    <xdr:ext cx="8659752" cy="6289408"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5615,18 +5689,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97EC1152-EA9A-43A3-9695-9B9EB129F172}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -5634,7 +5708,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5642,7 +5716,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5695,233 +5769,233 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>45</v>
+        <v>33.9</v>
       </c>
       <c r="C6">
-        <v>2.73</v>
+        <v>3.16</v>
       </c>
       <c r="D6">
-        <v>94.6</v>
+        <v>80.2</v>
       </c>
       <c r="E6">
-        <v>18.7</v>
+        <v>15.7</v>
       </c>
       <c r="F6">
-        <v>50</v>
+        <v>32.4</v>
       </c>
       <c r="G6">
-        <v>3.33</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>73.400000000000006</v>
+        <v>52.1</v>
       </c>
       <c r="I6">
-        <v>11.2</v>
+        <v>6.24</v>
       </c>
       <c r="J6">
-        <v>1.05</v>
+        <v>0.99</v>
       </c>
       <c r="K6">
-        <v>0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L6">
-        <v>22.9</v>
+        <v>1.98</v>
       </c>
       <c r="M6">
-        <v>13.2</v>
+        <v>1.04</v>
       </c>
       <c r="N6">
-        <v>7.11</v>
+        <v>7.1</v>
       </c>
       <c r="O6">
-        <v>0.72</v>
+        <v>0.83</v>
       </c>
       <c r="P6">
-        <v>15.8</v>
+        <v>15.5</v>
       </c>
       <c r="Q6">
-        <v>8.08</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>23.6</v>
+        <v>21.1</v>
       </c>
       <c r="C7">
-        <v>2.34</v>
+        <v>1.77</v>
       </c>
       <c r="D7">
-        <v>83</v>
+        <v>66.2</v>
       </c>
       <c r="E7">
-        <v>38.4</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="F7">
-        <v>77.599999999999994</v>
+        <v>20</v>
       </c>
       <c r="G7">
-        <v>5.58</v>
+        <v>2.33</v>
       </c>
       <c r="H7">
-        <v>78.400000000000006</v>
+        <v>78</v>
       </c>
       <c r="I7">
-        <v>43.2</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="J7">
-        <v>1.1000000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="K7">
-        <v>0.27</v>
+        <v>0.18</v>
       </c>
       <c r="L7">
-        <v>2.8</v>
+        <v>2.37</v>
       </c>
       <c r="M7">
-        <v>3.65</v>
+        <v>2.27</v>
       </c>
       <c r="N7">
-        <v>0.97</v>
+        <v>0.94</v>
       </c>
       <c r="O7">
-        <v>0.31</v>
+        <v>0.18</v>
       </c>
       <c r="P7">
-        <v>3.03</v>
+        <v>1.84</v>
       </c>
       <c r="Q7">
-        <v>3.33</v>
+        <v>1.94</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8">
-        <v>77.599999999999994</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="C8">
-        <v>5.58</v>
+        <v>5.12</v>
       </c>
       <c r="D8">
-        <v>78.400000000000006</v>
+        <v>435</v>
       </c>
       <c r="E8">
-        <v>43.2</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9">
-        <v>62</v>
+        <v>54.6</v>
       </c>
       <c r="C9">
-        <v>2.6</v>
+        <v>3.36</v>
       </c>
       <c r="D9">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E9">
-        <v>14.5</v>
+        <v>22.6</v>
       </c>
       <c r="F9">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G9">
-        <v>5.77</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="H9">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="I9">
-        <v>35.4</v>
+        <v>30</v>
       </c>
       <c r="J9">
-        <v>1.61</v>
+        <v>1.52</v>
       </c>
       <c r="K9">
-        <v>0.26</v>
+        <v>0.42</v>
       </c>
       <c r="L9">
-        <v>7.15</v>
+        <v>2.39</v>
       </c>
       <c r="M9">
-        <v>9.0500000000000007</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="N9">
-        <v>8.02</v>
+        <v>7.91</v>
       </c>
       <c r="O9">
-        <v>0.78</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P9">
-        <v>16.600000000000001</v>
+        <v>15.7</v>
       </c>
       <c r="Q9">
-        <v>7.92</v>
+        <v>5.09</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>87.4</v>
+        <v>72.3</v>
       </c>
       <c r="C10">
-        <v>4.5</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="D10">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="E10">
-        <v>27.6</v>
+        <v>31</v>
       </c>
       <c r="F10">
-        <v>85.3</v>
+        <v>75.099999999999994</v>
       </c>
       <c r="G10">
-        <v>7.62</v>
+        <v>12.2</v>
       </c>
       <c r="H10">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="I10">
-        <v>33.4</v>
+        <v>23.2</v>
       </c>
       <c r="J10">
-        <v>3.47</v>
+        <v>3.06</v>
       </c>
       <c r="K10">
-        <v>2.99</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L10">
-        <v>14.2</v>
+        <v>3.3</v>
       </c>
       <c r="M10">
-        <v>16.100000000000001</v>
+        <v>3.03</v>
       </c>
       <c r="N10">
-        <v>5.15</v>
+        <v>4.82</v>
       </c>
       <c r="O10">
-        <v>4.0599999999999996</v>
+        <v>5</v>
       </c>
       <c r="P10">
-        <v>10.3</v>
+        <v>3.1</v>
       </c>
       <c r="Q10">
-        <v>12.6</v>
+        <v>2.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>